<commit_message>
alterei o path do projeto e criei novo arquivo Sales Result
</commit_message>
<xml_diff>
--- a/Sales Results/Sales Results-2024-01-06.xlsx
+++ b/Sales Results/Sales Results-2024-01-06.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Adriano\Meus Arquivos\UiPath\Projetos\UipathAcademy\ExcelReportsConsolidation\Sales Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31AB381-4689-4241-935B-5A0D163729D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2E4782-AFE7-4257-8350-FF0C23E752D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3684" yWindow="1824" windowWidth="6468" windowHeight="8880" xr2:uid="{7FEDE06E-3E10-473A-A88D-EAF0D64CB1D9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="12576" xr2:uid="{7FEDE06E-3E10-473A-A88D-EAF0D64CB1D9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha2" sheetId="2" r:id="rId1"/>
-    <sheet name="Planilha1" sheetId="1" r:id="rId2"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -143,10 +143,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -367,16 +366,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>71120</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>78740</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>81280</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>370840</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -689,7 +688,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{37612769-333B-4976-B2AD-AB806E8ECB97}" name="SalesByStore" cacheId="2" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Dados" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{37612769-333B-4976-B2AD-AB806E8ECB97}" name="SalesByStore" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Dados" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1" chartFormat="1">
   <location ref="A1:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0" includeNewItemsInFilter="1">
@@ -1101,133 +1100,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38652D5C-8E6F-4E04-BF8E-8E57053A3A0F}">
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1">
-        <v>381.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1">
-        <v>922.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="1">
-        <v>745.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1">
-        <v>877.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="1">
-        <v>5637</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F40510C-0BE3-4124-804F-898A5FE6CC8B}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:D51"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1239,16 +1116,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1955,4 +1832,126 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38652D5C-8E6F-4E04-BF8E-8E57053A3A0F}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>381.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>922.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>745.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>877.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>5637</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>